<commit_message>
Update column names of text block templates spreadsheet
Enables easier comprehension of the data fields
</commit_message>
<xml_diff>
--- a/src/resources/templates/text_block_templates.xlsx
+++ b/src/resources/templates/text_block_templates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason D'Amico\Documents\cdf\pgov-cover-sheet-reader\src\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B6C7B5-592A-4FDC-B1CC-CF1CFAAEF53B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA5C773-4822-46AD-8037-97A38EB33537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,9 +28,6 @@
     <t>Context</t>
   </si>
   <si>
-    <t>Sentence Plural Template</t>
-  </si>
-  <si>
     <t>Summary_Report</t>
   </si>
   <si>
@@ -58,13 +55,16 @@
     <t>Currently in template</t>
   </si>
   <si>
-    <t>Variable In Code</t>
-  </si>
-  <si>
     <t>goal_status_breakdown_bullet</t>
   </si>
   <si>
     <t>Bullet point describing a each goal and its change quarter-over-quarter</t>
+  </si>
+  <si>
+    <t>Variable Name</t>
+  </si>
+  <si>
+    <t>Sentence Template Plural</t>
   </si>
 </sst>
 </file>
@@ -935,7 +935,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" activeCellId="1" sqref="A3:XFD3 A4:XFD4"/>
+      <selection activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -954,48 +954,48 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="144" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add speedometer_text entry to text block templates spreadsheet
</commit_message>
<xml_diff>
--- a/src/resources/templates/text_block_templates.xlsx
+++ b/src/resources/templates/text_block_templates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason D'Amico\Documents\cdf\pgov-cover-sheet-reader\src\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA5C773-4822-46AD-8037-97A38EB33537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92F85C1-4BFC-484C-A879-64B5EF807720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Template Document</t>
   </si>
@@ -43,6 +43,15 @@
     <t>**{APG name}**'s team identified the status of the goal as {previous goal status} this quarter, remaining consistent at its reported status of {current goal status} last quarter.</t>
   </si>
   <si>
+    <t>speedometer_text</t>
+  </si>
+  <si>
+    <t>APG_Summary</t>
+  </si>
+  <si>
+    <t>Underneath speedometer (current status) graphic on each APG page.</t>
+  </si>
+  <si>
     <t>**{APG name}**'s team identified the status of the goal as {previous goal status} this quarter, progressing from a status of {current goal status} last quarter.</t>
   </si>
   <si>
@@ -61,10 +70,16 @@
     <t>Bullet point describing a each goal and its change quarter-over-quarter</t>
   </si>
   <si>
+    <t>The goal team reported this goal as **{status}** of its expected progression in {quarter} {year}.</t>
+  </si>
+  <si>
     <t>Variable Name</t>
   </si>
   <si>
     <t>Sentence Template Plural</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -932,10 +947,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -954,7 +969,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -963,7 +978,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>4</v>
@@ -972,7 +987,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="144" x14ac:dyDescent="0.3">
@@ -980,22 +995,39 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement text template from Excel sheet for speedometer summary text (#77)
* Add speedometer_text entry to text block templates spreadsheet

* Implement text block template population for speedometer text

* Remove (now unnecessary) creation of new RichText object
</commit_message>
<xml_diff>
--- a/src/resources/templates/text_block_templates.xlsx
+++ b/src/resources/templates/text_block_templates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason D'Amico\Documents\cdf\pgov-cover-sheet-reader\src\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA5C773-4822-46AD-8037-97A38EB33537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92F85C1-4BFC-484C-A879-64B5EF807720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Template Document</t>
   </si>
@@ -43,6 +43,15 @@
     <t>**{APG name}**'s team identified the status of the goal as {previous goal status} this quarter, remaining consistent at its reported status of {current goal status} last quarter.</t>
   </si>
   <si>
+    <t>speedometer_text</t>
+  </si>
+  <si>
+    <t>APG_Summary</t>
+  </si>
+  <si>
+    <t>Underneath speedometer (current status) graphic on each APG page.</t>
+  </si>
+  <si>
     <t>**{APG name}**'s team identified the status of the goal as {previous goal status} this quarter, progressing from a status of {current goal status} last quarter.</t>
   </si>
   <si>
@@ -61,10 +70,16 @@
     <t>Bullet point describing a each goal and its change quarter-over-quarter</t>
   </si>
   <si>
+    <t>The goal team reported this goal as **{status}** of its expected progression in {quarter} {year}.</t>
+  </si>
+  <si>
     <t>Variable Name</t>
   </si>
   <si>
     <t>Sentence Template Plural</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -932,10 +947,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -954,7 +969,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -963,7 +978,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>4</v>
@@ -972,7 +987,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="144" x14ac:dyDescent="0.3">
@@ -980,22 +995,39 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create text block template entry for recurring challenge
</commit_message>
<xml_diff>
--- a/src/resources/templates/text_block_templates.xlsx
+++ b/src/resources/templates/text_block_templates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason D'Amico\Documents\cdf\pgov-cover-sheet-reader\src\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92F85C1-4BFC-484C-A879-64B5EF807720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23131A28-33F8-4D44-AA68-55C3790B6D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Template Document</t>
   </si>
@@ -80,6 +80,15 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>One feature of the auto-generated template is that it pulls the most common recurring challenges across the agency. This text block summarizes how many times a recurring challenge has occurred for a given agency.</t>
+  </si>
+  <si>
+    <t>recurring_challenge_text</t>
+  </si>
+  <si>
+    <t>**{challenge}** has been reported as challenge for the **{goal}** team in each of the last **{challenge count} quarters**.</t>
   </si>
 </sst>
 </file>
@@ -947,10 +956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1013,20 +1022,34 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implement text template from Excel sheet for recurring challenges text (#78)
* Create text block template entry for recurring challenge

* Add function to retrieve the recurring challenges text template

Note that the function takes arguments specific to the recurring challenge rather than receiving an agency object and subsequently retrieving the top recurring challenges.

* Implement function that retrieves text template into dynamic text filling

* Update summary report template with updated recurring challenges keywords
</commit_message>
<xml_diff>
--- a/src/resources/templates/text_block_templates.xlsx
+++ b/src/resources/templates/text_block_templates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason D'Amico\Documents\cdf\pgov-cover-sheet-reader\src\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92F85C1-4BFC-484C-A879-64B5EF807720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23131A28-33F8-4D44-AA68-55C3790B6D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Template Document</t>
   </si>
@@ -80,6 +80,15 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>One feature of the auto-generated template is that it pulls the most common recurring challenges across the agency. This text block summarizes how many times a recurring challenge has occurred for a given agency.</t>
+  </si>
+  <si>
+    <t>recurring_challenge_text</t>
+  </si>
+  <si>
+    <t>**{challenge}** has been reported as challenge for the **{goal}** team in each of the last **{challenge count} quarters**.</t>
   </si>
 </sst>
 </file>
@@ -947,10 +956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1013,20 +1022,34 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>